<commit_message>
Added code for updating email bounce status
</commit_message>
<xml_diff>
--- a/files/excel/CMPG-A1-LD2-11122025.xlsx
+++ b/files/excel/CMPG-A1-LD2-11122025.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -65,6 +65,18 @@
       <family val="2"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <color rgb="FF0072C6"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="4">
@@ -130,7 +142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -150,6 +162,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -228,9 +242,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -268,7 +282,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -374,7 +388,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -516,7 +530,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -529,21 +543,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:O96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="18.21875" customWidth="1" min="1" max="1"/>
-    <col width="52.21875" customWidth="1" min="2" max="2"/>
-    <col width="20.5546875" customWidth="1" min="4" max="4"/>
-    <col width="17.44140625" customWidth="1" min="5" max="5"/>
-    <col width="39.88671875" customWidth="1" min="6" max="6"/>
-    <col width="25.5546875" customWidth="1" min="7" max="7"/>
-    <col width="29.77734375" customWidth="1" min="8" max="8"/>
+    <col width="18.28515625" customWidth="1" min="1" max="1"/>
+    <col width="52.28515625" customWidth="1" min="2" max="2"/>
+    <col width="20.5703125" customWidth="1" min="4" max="4"/>
+    <col width="17.42578125" customWidth="1" min="5" max="5"/>
+    <col width="39.85546875" customWidth="1" min="6" max="6"/>
+    <col width="25.5703125" customWidth="1" min="7" max="7"/>
+    <col width="32.140625" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="24.42578125" customWidth="1" min="9" max="9"/>
+    <col width="37.42578125" bestFit="1" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -569,6 +585,11 @@
           <t>CMPG-11122025.html</t>
         </is>
       </c>
+      <c r="O2" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">saumya.gupta@aisglass.com </t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -581,6 +602,11 @@
           <t xml:space="preserve"> Support Your Team’s Growth with Better Learning</t>
         </is>
       </c>
+      <c r="O3" s="4" t="inlineStr">
+        <is>
+          <t>apoorva.patil@tcs.com</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="C4" s="2" t="inlineStr">
@@ -611,6 +637,16 @@
       <c r="H4" s="2" t="inlineStr">
         <is>
           <t>Status</t>
+        </is>
+      </c>
+      <c r="I4" s="2" t="inlineStr">
+        <is>
+          <t>Bounce back</t>
+        </is>
+      </c>
+      <c r="O4" s="4" t="inlineStr">
+        <is>
+          <t>prashant.kothari@airindiaexpress.in</t>
         </is>
       </c>
     </row>
@@ -640,7 +676,15 @@
       </c>
       <c r="H5" s="3" t="inlineStr">
         <is>
-          <t>Sent email at slno 1 at time: 11/12/2025,17:54:15</t>
+          <t>Sent email at 08/12/2025,13:19:32</t>
+        </is>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="4" t="inlineStr">
+        <is>
+          <t>nidhika.abrol@rjcorp.in</t>
         </is>
       </c>
     </row>
@@ -670,11 +714,19 @@
       </c>
       <c r="H6" s="3" t="inlineStr">
         <is>
-          <t>Sent email at slno 2 at time: 11/12/2025,17:54:23</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1" thickBot="1">
+          <t>Sent email at 08/12/2025,13:19:37</t>
+        </is>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" s="4" t="inlineStr">
+        <is>
+          <t>monideepa.j@tataconsumer.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1" thickBot="1">
       <c r="C7" s="3" t="n">
         <v>3</v>
       </c>
@@ -695,11 +747,19 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Sent email at slno 3 at time: 11/12/2025,17:58:16</t>
-        </is>
-      </c>
-    </row>
-    <row r="8" ht="15" customHeight="1" thickBot="1">
+          <t>Updated bounce status of email at slno 3</t>
+        </is>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" s="4" t="inlineStr">
+        <is>
+          <t>rkc@apac.ko.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1" thickBot="1">
       <c r="C8" s="3" t="n">
         <v>4</v>
       </c>
@@ -720,11 +780,19 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Sent email at slno 4 at time: 11/12/2025,17:58:23</t>
-        </is>
-      </c>
-    </row>
-    <row r="9" ht="15" customHeight="1" thickBot="1">
+          <t>Updated bounce status of email at slno 4</t>
+        </is>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="O8" s="4" t="inlineStr">
+        <is>
+          <t>vishal.dey@hdfcergo.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1" thickBot="1">
       <c r="C9" s="3" t="n">
         <v>5</v>
       </c>
@@ -743,13 +811,16 @@
           <t>akshay.mutha@microland.com</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Sent email at slno 5 at time: 11/12/2025,17:58:28</t>
-        </is>
-      </c>
-    </row>
-    <row r="10" ht="15" customHeight="1" thickBot="1">
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" s="11" t="inlineStr">
+        <is>
+          <t>manjirika.vivalkar@neo-soft.fr</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1" thickBot="1">
       <c r="C10" s="3" t="n">
         <v>6</v>
       </c>
@@ -768,13 +839,16 @@
           <t>saumya.gupta@aisglass.com</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Sent email at slno 6 at time: 11/12/2025,17:58:33</t>
-        </is>
-      </c>
-    </row>
-    <row r="11" ht="15" customHeight="1" thickBot="1">
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" s="4" t="inlineStr">
+        <is>
+          <t>meenal.gupta@bajajallianz.co.in</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1" thickBot="1">
       <c r="C11" s="3" t="n">
         <v>7</v>
       </c>
@@ -793,13 +867,16 @@
           <t>sridhar.c@in.bosch.com</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Sent email at slno 7 at time: 11/12/2025,17:58:38</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="15" customHeight="1" thickBot="1">
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="O11" s="4" t="inlineStr">
+        <is>
+          <t>vishwachandrannair@iiflsamasta.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1" thickBot="1">
       <c r="C12" s="3" t="n">
         <v>8</v>
       </c>
@@ -814,13 +891,16 @@
           <t>m@capgemini.com</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Sent email at slno 8 at time: 11/12/2025,17:58:43</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" ht="15" customHeight="1" thickBot="1">
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O12" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> rajeshs@equitas.in </t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1" thickBot="1">
       <c r="C13" s="3" t="n">
         <v>9</v>
       </c>
@@ -839,13 +919,16 @@
           <t>naveen_sridhar@comcast.com</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Sent email at slno 9 at time: 11/12/2025,17:58:50</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="15" customHeight="1" thickBot="1">
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4" t="inlineStr">
+        <is>
+          <t>rishi.raghuvanshi@ujjivan.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1" thickBot="1">
       <c r="C14" s="3" t="n">
         <v>10</v>
       </c>
@@ -864,13 +947,16 @@
           <t>apoorva.patil@tcs.com</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Sent email at slno 10 at time: 11/12/2025,17:58:54</t>
-        </is>
-      </c>
-    </row>
-    <row r="15" ht="15" customHeight="1" thickBot="1">
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">rohith.reghunadhan@axisbank.com </t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1" thickBot="1">
       <c r="C15" s="3" t="n">
         <v>11</v>
       </c>
@@ -889,13 +975,16 @@
           <t>plole@deloitte.com</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Sent email at slno 11 at time: 11/12/2025,17:58:59</t>
-        </is>
-      </c>
-    </row>
-    <row r="16" ht="15" customHeight="1" thickBot="1">
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4" t="inlineStr">
+        <is>
+          <t>raghavg@vfsglobal.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1" thickBot="1">
       <c r="C16" s="3" t="n">
         <v>12</v>
       </c>
@@ -914,13 +1003,11 @@
           <t>nishanth.dasari@berkadia.com</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Sent email at slno 12 at time: 11/12/2025,17:59:04</t>
-        </is>
-      </c>
-    </row>
-    <row r="17" ht="15" customHeight="1" thickBot="1">
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" customHeight="1" thickBot="1">
       <c r="C17" s="3" t="n">
         <v>13</v>
       </c>
@@ -939,13 +1026,11 @@
           <t>nitisha.jain@entigrity.com</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Sent email at slno 13 at time: 11/12/2025,17:59:10</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" ht="15" customHeight="1" thickBot="1">
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1" thickBot="1">
       <c r="C18" s="3" t="n">
         <v>14</v>
       </c>
@@ -964,13 +1049,11 @@
           <t>zain@redefineservice.in</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Sent email at slno 14 at time: 11/12/2025,17:59:15</t>
-        </is>
-      </c>
-    </row>
-    <row r="19" ht="15" customHeight="1" thickBot="1">
+      <c r="I18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1" thickBot="1">
       <c r="C19" s="3" t="n">
         <v>15</v>
       </c>
@@ -989,13 +1072,11 @@
           <t>jyotesh.singh@spectraforce.com</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Sent email at slno 15 at time: 11/12/2025,17:59:19</t>
-        </is>
-      </c>
-    </row>
-    <row r="20" ht="15" customHeight="1" thickBot="1">
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" customHeight="1" thickBot="1">
       <c r="C20" s="3" t="n">
         <v>16</v>
       </c>
@@ -1014,13 +1095,11 @@
           <t>ritika.malhotra@maxestates.in</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Sent email at slno 16 at time: 11/12/2025,17:59:25</t>
-        </is>
-      </c>
-    </row>
-    <row r="21" ht="15" customHeight="1" thickBot="1">
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1" thickBot="1">
       <c r="C21" s="3" t="n">
         <v>17</v>
       </c>
@@ -1039,13 +1118,11 @@
           <t>priyanka.hazra@cognizant.com</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Sent email at slno 17 at time: 11/12/2025,17:59:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="22" ht="15" customHeight="1" thickBot="1">
+      <c r="I21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" thickBot="1">
       <c r="C22" s="3" t="n">
         <v>18</v>
       </c>
@@ -1064,13 +1141,11 @@
           <t>radhika.kadam@assurant.com</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Sent email at slno 18 at time: 11/12/2025,17:59:36</t>
-        </is>
-      </c>
-    </row>
-    <row r="23" ht="15" customHeight="1" thickBot="1">
+      <c r="I22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" customHeight="1" thickBot="1">
       <c r="C23" s="3" t="n">
         <v>19</v>
       </c>
@@ -1089,13 +1164,11 @@
           <t>aman.12322434@lpu.in</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>Sent email at slno 19 at time: 11/12/2025,17:59:44</t>
-        </is>
-      </c>
-    </row>
-    <row r="24" ht="15" customHeight="1" thickBot="1">
+      <c r="I23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1" thickBot="1">
       <c r="C24" s="3" t="n">
         <v>20</v>
       </c>
@@ -1114,13 +1187,11 @@
           <t>ashutosh.shinde@henkel.com</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>Sent email at slno 20 at time: 11/12/2025,17:59:49</t>
-        </is>
-      </c>
-    </row>
-    <row r="25" ht="15" customHeight="1" thickBot="1">
+      <c r="I24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" customHeight="1" thickBot="1">
       <c r="C25" s="3" t="n">
         <v>21</v>
       </c>
@@ -1139,13 +1210,11 @@
           <t>pravin.tekade@netcracker.com</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>Sent email at slno 21 at time: 11/12/2025,17:59:58</t>
-        </is>
-      </c>
-    </row>
-    <row r="26" ht="15" customHeight="1" thickBot="1">
+      <c r="I25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" ht="15.75" customHeight="1" thickBot="1">
       <c r="C26" s="3" t="n">
         <v>22</v>
       </c>
@@ -1164,13 +1233,11 @@
           <t>hema.nalini@microchip.com</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>Sent email at slno 22 at time: 11/12/2025,18:00:02</t>
-        </is>
-      </c>
-    </row>
-    <row r="27" ht="15" customHeight="1" thickBot="1">
+      <c r="I26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1" thickBot="1">
       <c r="C27" s="3" t="n">
         <v>23</v>
       </c>
@@ -1189,13 +1256,11 @@
           <t>g.sharma@yesbank.in</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>Sent email at slno 23 at time: 11/12/2025,18:00:07</t>
-        </is>
-      </c>
-    </row>
-    <row r="28" ht="15" customHeight="1" thickBot="1">
+      <c r="I27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1" thickBot="1">
       <c r="C28" s="3" t="n">
         <v>24</v>
       </c>
@@ -1214,13 +1279,11 @@
           <t>aman.nanda@hdbfs.com</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Sent email at slno 24 at time: 11/12/2025,18:00:12</t>
-        </is>
-      </c>
-    </row>
-    <row r="29" ht="15" customHeight="1" thickBot="1">
+      <c r="I28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" ht="15.75" customHeight="1" thickBot="1">
       <c r="C29" s="3" t="n">
         <v>25</v>
       </c>
@@ -1239,13 +1302,11 @@
           <t>pritam.gangwal@croma.gr</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>Sent email at slno 25 at time: 11/12/2025,18:00:18</t>
-        </is>
-      </c>
-    </row>
-    <row r="30" ht="15" customHeight="1" thickBot="1">
+      <c r="I29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" ht="15.75" customHeight="1" thickBot="1">
       <c r="C30" s="3" t="n">
         <v>26</v>
       </c>
@@ -1264,13 +1325,11 @@
           <t>ishani.sengupta@bandhanbank.com</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>Sent email at slno 26 at time: 11/12/2025,18:00:22</t>
-        </is>
-      </c>
-    </row>
-    <row r="31" ht="15" customHeight="1" thickBot="1">
+      <c r="I30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1" thickBot="1">
       <c r="C31" s="3" t="n">
         <v>27</v>
       </c>
@@ -1289,13 +1348,11 @@
           <t>chiragshiv@smcindiaonline.com</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>Sent email at slno 27 at time: 11/12/2025,18:00:27</t>
-        </is>
-      </c>
-    </row>
-    <row r="32" ht="15" customHeight="1" thickBot="1">
+      <c r="I31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" ht="15.75" customHeight="1" thickBot="1">
       <c r="C32" s="3" t="n">
         <v>28</v>
       </c>
@@ -1314,13 +1371,11 @@
           <t>dwiti.rathod@analytix.com</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>Sent email at slno 28 at time: 11/12/2025,18:00:33</t>
-        </is>
-      </c>
-    </row>
-    <row r="33" ht="15" customHeight="1" thickBot="1">
+      <c r="I32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" ht="15.75" customHeight="1" thickBot="1">
       <c r="C33" s="3" t="n">
         <v>29</v>
       </c>
@@ -1339,13 +1394,11 @@
           <t>samreen@cetpainfotech.com</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>Sent email at slno 29 at time: 11/12/2025,18:00:38</t>
-        </is>
-      </c>
-    </row>
-    <row r="34" ht="15" customHeight="1" thickBot="1">
+      <c r="I33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75" customHeight="1" thickBot="1">
       <c r="C34" s="3" t="n">
         <v>30</v>
       </c>
@@ -1364,13 +1417,11 @@
           <t>radhika.annapragada@perceptive.com</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>Sent email at slno 30 at time: 11/12/2025,18:00:44</t>
-        </is>
-      </c>
-    </row>
-    <row r="35" ht="15" customHeight="1" thickBot="1">
+      <c r="I34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1" thickBot="1">
       <c r="C35" s="3" t="n">
         <v>31</v>
       </c>
@@ -1389,13 +1440,11 @@
           <t>prashant.kothari@airindiaexpress.in</t>
         </is>
       </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>Sent email at slno 31 at time: 11/12/2025,18:00:49</t>
-        </is>
-      </c>
-    </row>
-    <row r="36" ht="15" customHeight="1" thickBot="1">
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" ht="15.75" customHeight="1" thickBot="1">
       <c r="C36" s="3" t="n">
         <v>32</v>
       </c>
@@ -1414,13 +1463,11 @@
           <t>mdcunha@alkylamines.com</t>
         </is>
       </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>Sent email at slno 32 at time: 11/12/2025,18:00:54</t>
-        </is>
-      </c>
-    </row>
-    <row r="37" ht="15" customHeight="1" thickBot="1">
+      <c r="I36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" ht="15.75" customHeight="1" thickBot="1">
       <c r="C37" s="3" t="n">
         <v>33</v>
       </c>
@@ -1439,13 +1486,11 @@
           <t>nigel.dyas@id-medical.com</t>
         </is>
       </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>Sent email at slno 33 at time: 11/12/2025,18:01:02</t>
-        </is>
-      </c>
-    </row>
-    <row r="38" ht="15" customHeight="1" thickBot="1">
+      <c r="I37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" ht="15.75" customHeight="1" thickBot="1">
       <c r="C38" s="3" t="n">
         <v>34</v>
       </c>
@@ -1464,13 +1509,11 @@
           <t>parthadas@waaree.com</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>Sent email at slno 34 at time: 11/12/2025,18:01:07</t>
-        </is>
-      </c>
-    </row>
-    <row r="39" ht="15" customHeight="1" thickBot="1">
+      <c r="I38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" ht="15.75" customHeight="1" thickBot="1">
       <c r="C39" s="3" t="n">
         <v>35</v>
       </c>
@@ -1489,13 +1532,11 @@
           <t>rohit.negi@ness.com</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Sent email at slno 35 at time: 11/12/2025,18:01:12</t>
-        </is>
-      </c>
-    </row>
-    <row r="40" ht="15" customHeight="1" thickBot="1">
+      <c r="I39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" ht="15.75" customHeight="1" thickBot="1">
       <c r="C40" s="3" t="n">
         <v>36</v>
       </c>
@@ -1514,13 +1555,11 @@
           <t>nikhil.jaiswal@swastika.co.in</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>Sent email at slno 36 at time: 11/12/2025,18:01:17</t>
-        </is>
-      </c>
-    </row>
-    <row r="41" ht="15" customHeight="1" thickBot="1">
+      <c r="I40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" ht="15.75" customHeight="1" thickBot="1">
       <c r="C41" s="3" t="n">
         <v>37</v>
       </c>
@@ -1539,13 +1578,11 @@
           <t>manjirika.vivalkar@neo-soft.fr</t>
         </is>
       </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>Sent email at slno 37 at time: 11/12/2025,18:01:23</t>
-        </is>
-      </c>
-    </row>
-    <row r="42" ht="15" customHeight="1" thickBot="1">
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" ht="15.75" customHeight="1" thickBot="1">
       <c r="C42" s="3" t="n">
         <v>38</v>
       </c>
@@ -1564,13 +1601,11 @@
           <t>ojhapuskar@gmail.com</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>Sent email at slno 38 at time: 11/12/2025,18:01:27</t>
-        </is>
-      </c>
-    </row>
-    <row r="43" ht="15" customHeight="1" thickBot="1">
+      <c r="I42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" ht="15.75" customHeight="1" thickBot="1">
       <c r="C43" s="3" t="n">
         <v>39</v>
       </c>
@@ -1589,13 +1624,11 @@
           <t>pavan.kalyan@groupbayport.com</t>
         </is>
       </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>Sent email at slno 39 at time: 11/12/2025,18:01:34</t>
-        </is>
-      </c>
-    </row>
-    <row r="44" ht="15" customHeight="1" thickBot="1">
+      <c r="I43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" ht="15.75" customHeight="1" thickBot="1">
       <c r="C44" s="3" t="n">
         <v>40</v>
       </c>
@@ -1614,13 +1647,11 @@
           <t>meenal.gupta@bajajallianz.co.in</t>
         </is>
       </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>Sent email at slno 40 at time: 11/12/2025,18:01:39</t>
-        </is>
-      </c>
-    </row>
-    <row r="45" ht="15" customHeight="1" thickBot="1">
+      <c r="I44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" ht="15.75" customHeight="1" thickBot="1">
       <c r="C45" s="3" t="n">
         <v>41</v>
       </c>
@@ -1639,13 +1670,11 @@
           <t>gaurav.mehta@danone.com</t>
         </is>
       </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>Sent email at slno 41 at time: 11/12/2025,18:01:44</t>
-        </is>
-      </c>
-    </row>
-    <row r="46" ht="15" customHeight="1" thickBot="1">
+      <c r="I45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" ht="15.75" customHeight="1" thickBot="1">
       <c r="C46" s="3" t="n">
         <v>42</v>
       </c>
@@ -1664,13 +1693,11 @@
           <t>deepak.chandola@unilever.com</t>
         </is>
       </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>Sent email at slno 42 at time: 11/12/2025,18:01:49</t>
-        </is>
-      </c>
-    </row>
-    <row r="47" ht="15" customHeight="1" thickBot="1">
+      <c r="I46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" ht="15.75" customHeight="1" thickBot="1">
       <c r="C47" s="3" t="n">
         <v>43</v>
       </c>
@@ -1689,13 +1716,11 @@
           <t>jagtianineha@gmail.com</t>
         </is>
       </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>Sent email at slno 43 at time: 11/12/2025,18:01:54</t>
-        </is>
-      </c>
-    </row>
-    <row r="48" ht="15" customHeight="1" thickBot="1">
+      <c r="I47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" ht="15.75" customHeight="1" thickBot="1">
       <c r="C48" s="3" t="n">
         <v>44</v>
       </c>
@@ -1714,13 +1739,11 @@
           <t>hasan.siddique@hotmail.com</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>Sent email at slno 44 at time: 11/12/2025,18:01:59</t>
-        </is>
-      </c>
-    </row>
-    <row r="49" ht="15" customHeight="1" thickBot="1">
+      <c r="I48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" ht="15.75" customHeight="1" thickBot="1">
       <c r="C49" s="3" t="n">
         <v>45</v>
       </c>
@@ -1739,13 +1762,11 @@
           <t>nidhika.abrol@rjcorp.in</t>
         </is>
       </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>Sent email at slno 45 at time: 11/12/2025,18:02:04</t>
-        </is>
-      </c>
-    </row>
-    <row r="50" ht="15" customHeight="1" thickBot="1">
+      <c r="I49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" ht="15.75" customHeight="1" thickBot="1">
       <c r="C50" s="3" t="n">
         <v>46</v>
       </c>
@@ -1764,13 +1785,11 @@
           <t>monideepa.j@tataconsumer.com</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>Sent email at slno 46 at time: 11/12/2025,18:02:08</t>
-        </is>
-      </c>
-    </row>
-    <row r="51" ht="15" customHeight="1" thickBot="1">
+      <c r="I50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" ht="15.75" customHeight="1" thickBot="1">
       <c r="C51" s="3" t="n">
         <v>47</v>
       </c>
@@ -1789,13 +1808,11 @@
           <t>siddhesh.ajgaonkar@marico.com</t>
         </is>
       </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>Sent email at slno 47 at time: 11/12/2025,18:02:14</t>
-        </is>
-      </c>
-    </row>
-    <row r="52" ht="15" customHeight="1" thickBot="1">
+      <c r="I51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" ht="15.75" customHeight="1" thickBot="1">
       <c r="C52" s="3" t="n">
         <v>48</v>
       </c>
@@ -1814,13 +1831,11 @@
           <t>kanchan_balani@colpal.com</t>
         </is>
       </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>Sent email at slno 48 at time: 11/12/2025,18:02:18</t>
-        </is>
-      </c>
-    </row>
-    <row r="53" ht="15" customHeight="1" thickBot="1">
+      <c r="I52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" ht="15.75" customHeight="1" thickBot="1">
       <c r="C53" s="3" t="n">
         <v>49</v>
       </c>
@@ -1839,13 +1854,11 @@
           <t>rkc@apac.ko.com</t>
         </is>
       </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>Sent email at slno 49 at time: 11/12/2025,18:02:23</t>
-        </is>
-      </c>
-    </row>
-    <row r="54" ht="15" customHeight="1" thickBot="1">
+      <c r="I53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" ht="15.75" customHeight="1" thickBot="1">
       <c r="C54" s="3" t="n">
         <v>50</v>
       </c>
@@ -1864,13 +1877,11 @@
           <t>paramita.nanda@pepsico.com</t>
         </is>
       </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>Sent email at slno 50 at time: 11/12/2025,18:02:28</t>
-        </is>
-      </c>
-    </row>
-    <row r="55" ht="15" customHeight="1" thickBot="1">
+      <c r="I54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" ht="15.75" customHeight="1" thickBot="1">
       <c r="C55" s="3" t="n">
         <v>51</v>
       </c>
@@ -1889,13 +1900,11 @@
           <t>shreyaskarle09@gmail.com</t>
         </is>
       </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>Sent email at slno 51 at time: 11/12/2025,18:02:33</t>
-        </is>
-      </c>
-    </row>
-    <row r="56" ht="15" customHeight="1" thickBot="1">
+      <c r="I55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" ht="15.75" customHeight="1" thickBot="1">
       <c r="C56" s="3" t="n">
         <v>52</v>
       </c>
@@ -1914,13 +1923,11 @@
           <t>preety.dhanvijay@parle.biz</t>
         </is>
       </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>Sent email at slno 52 at time: 11/12/2025,18:02:38</t>
-        </is>
-      </c>
-    </row>
-    <row r="57" ht="15" customHeight="1" thickBot="1">
+      <c r="I56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" ht="15.75" customHeight="1" thickBot="1">
       <c r="C57" s="3" t="n">
         <v>53</v>
       </c>
@@ -1939,13 +1946,11 @@
           <t>neha.somani@zyduscadila.com</t>
         </is>
       </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>Sent email at slno 53 at time: 11/12/2025,18:02:42</t>
-        </is>
-      </c>
-    </row>
-    <row r="58" ht="15" customHeight="1" thickBot="1">
+      <c r="I57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" ht="15.75" customHeight="1" thickBot="1">
       <c r="C58" s="3" t="n">
         <v>54</v>
       </c>
@@ -1964,13 +1969,11 @@
           <t>vishal.dey@hdfcergo.com</t>
         </is>
       </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>Sent email at slno 54 at time: 11/12/2025,18:02:47</t>
-        </is>
-      </c>
-    </row>
-    <row r="59" ht="15" customHeight="1" thickBot="1">
+      <c r="I58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" ht="15.75" customHeight="1" thickBot="1">
       <c r="C59" s="3" t="n">
         <v>55</v>
       </c>
@@ -1989,13 +1992,11 @@
           <t>robin.ganjoo@genpact.com</t>
         </is>
       </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>Sent email at slno 55 at time: 11/12/2025,18:02:52</t>
-        </is>
-      </c>
-    </row>
-    <row r="60" ht="15" customHeight="1" thickBot="1">
+      <c r="I59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" ht="15.75" customHeight="1" thickBot="1">
       <c r="C60" s="3" t="n">
         <v>56</v>
       </c>
@@ -2014,13 +2015,11 @@
           <t>namrata.doshi@homefirstindia.com</t>
         </is>
       </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>Sent email at slno 56 at time: 11/12/2025,18:02:59</t>
-        </is>
-      </c>
-    </row>
-    <row r="61" ht="15" customHeight="1" thickBot="1">
+      <c r="I60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" ht="15.75" customHeight="1" thickBot="1">
       <c r="C61" s="3" t="n">
         <v>57</v>
       </c>
@@ -2039,13 +2038,11 @@
           <t>manojbhattacharya@teletech.com</t>
         </is>
       </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>Sent email at slno 57 at time: 11/12/2025,18:03:07</t>
-        </is>
-      </c>
-    </row>
-    <row r="62" ht="15" customHeight="1" thickBot="1">
+      <c r="I61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" ht="15.75" customHeight="1" thickBot="1">
       <c r="C62" s="3" t="n">
         <v>58</v>
       </c>
@@ -2064,13 +2061,11 @@
           <t>rajeshs@equitas.in</t>
         </is>
       </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>Sent email at slno 58 at time: 11/12/2025,18:03:12</t>
-        </is>
-      </c>
-    </row>
-    <row r="63" ht="15" customHeight="1" thickBot="1">
+      <c r="I62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" ht="15.75" customHeight="1" thickBot="1">
       <c r="C63" s="3" t="n">
         <v>59</v>
       </c>
@@ -2089,13 +2084,11 @@
           <t>vishwachandrannair@iiflsamasta.com</t>
         </is>
       </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>Sent email at slno 59 at time: 11/12/2025,18:03:18</t>
-        </is>
-      </c>
-    </row>
-    <row r="64" ht="15" customHeight="1" thickBot="1">
+      <c r="I63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" ht="15.75" customHeight="1" thickBot="1">
       <c r="C64" s="3" t="n">
         <v>60</v>
       </c>
@@ -2114,13 +2107,11 @@
           <t>aradhana.pandey@kfintech.com</t>
         </is>
       </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>Sent email at slno 60 at time: 11/12/2025,18:03:23</t>
-        </is>
-      </c>
-    </row>
-    <row r="65" ht="15" customHeight="1" thickBot="1">
+      <c r="I64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" ht="15.75" customHeight="1" thickBot="1">
       <c r="C65" s="3" t="n">
         <v>61</v>
       </c>
@@ -2139,13 +2130,11 @@
           <t>neelam.mehrawat@bandhanbank.com</t>
         </is>
       </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>Sent email at slno 61 at time: 11/12/2025,18:03:27</t>
-        </is>
-      </c>
-    </row>
-    <row r="66" ht="15" customHeight="1" thickBot="1">
+      <c r="I65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" ht="15.75" customHeight="1" thickBot="1">
       <c r="C66" s="3" t="n">
         <v>62</v>
       </c>
@@ -2164,13 +2153,11 @@
           <t>nsonawadekar@nse.co.in</t>
         </is>
       </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>Sent email at slno 62 at time: 11/12/2025,18:03:32</t>
-        </is>
-      </c>
-    </row>
-    <row r="67" ht="15" customHeight="1" thickBot="1">
+      <c r="I66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" ht="15.75" customHeight="1" thickBot="1">
       <c r="C67" s="3" t="n">
         <v>63</v>
       </c>
@@ -2189,13 +2176,11 @@
           <t>rishi.raghuvanshi@ujjivan.com</t>
         </is>
       </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>Sent email at slno 63 at time: 11/12/2025,18:03:37</t>
-        </is>
-      </c>
-    </row>
-    <row r="68" ht="15" customHeight="1" thickBot="1">
+      <c r="I67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" ht="15.75" customHeight="1" thickBot="1">
       <c r="C68" s="3" t="n">
         <v>64</v>
       </c>
@@ -2214,13 +2199,11 @@
           <t>rakesh.pal@axisbank.com</t>
         </is>
       </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>Sent email at slno 64 at time: 11/12/2025,18:03:43</t>
-        </is>
-      </c>
-    </row>
-    <row r="69" ht="15" customHeight="1" thickBot="1">
+      <c r="I68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" ht="15.75" customHeight="1" thickBot="1">
       <c r="C69" s="3" t="n">
         <v>65</v>
       </c>
@@ -2239,13 +2222,11 @@
           <t>ruchijoshi@hdfcsales.com</t>
         </is>
       </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>Sent email at slno 65 at time: 11/12/2025,18:03:48</t>
-        </is>
-      </c>
-    </row>
-    <row r="70" ht="15" customHeight="1" thickBot="1">
+      <c r="I69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" ht="15.75" customHeight="1" thickBot="1">
       <c r="C70" s="3" t="n">
         <v>66</v>
       </c>
@@ -2264,13 +2245,11 @@
           <t>jyothirmaie.suresh@allianz.com</t>
         </is>
       </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>Sent email at slno 66 at time: 11/12/2025,18:03:53</t>
-        </is>
-      </c>
-    </row>
-    <row r="71" ht="15" customHeight="1" thickBot="1">
+      <c r="I70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" ht="15.75" customHeight="1" thickBot="1">
       <c r="C71" s="3" t="n">
         <v>67</v>
       </c>
@@ -2289,13 +2268,11 @@
           <t>nishka.prabha@bajajfinserv.in</t>
         </is>
       </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>Sent email at slno 67 at time: 11/12/2025,18:03:58</t>
-        </is>
-      </c>
-    </row>
-    <row r="72" ht="15" customHeight="1" thickBot="1">
+      <c r="I71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" ht="15.75" customHeight="1" thickBot="1">
       <c r="C72" s="3" t="n">
         <v>68</v>
       </c>
@@ -2314,13 +2291,11 @@
           <t>sunny.thakur@aubank.in</t>
         </is>
       </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>Sent email at slno 68 at time: 11/12/2025,18:04:03</t>
-        </is>
-      </c>
-    </row>
-    <row r="73" ht="15" customHeight="1" thickBot="1">
+      <c r="I72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" ht="15.75" customHeight="1" thickBot="1">
       <c r="C73" s="3" t="n">
         <v>69</v>
       </c>
@@ -2339,13 +2314,11 @@
           <t>shiti.nanda@ujjivan.com</t>
         </is>
       </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>Sent email at slno 69 at time: 11/12/2025,18:04:08</t>
-        </is>
-      </c>
-    </row>
-    <row r="74" ht="15" customHeight="1" thickBot="1">
+      <c r="I73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" ht="15.75" customHeight="1" thickBot="1">
       <c r="C74" s="3" t="n">
         <v>70</v>
       </c>
@@ -2364,13 +2337,11 @@
           <t>chiquitta.dmello@bajajfinserv.in</t>
         </is>
       </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>Sent email at slno 70 at time: 11/12/2025,18:04:15</t>
-        </is>
-      </c>
-    </row>
-    <row r="75" ht="15" customHeight="1" thickBot="1">
+      <c r="I74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" ht="15.75" customHeight="1" thickBot="1">
       <c r="C75" s="3" t="n">
         <v>71</v>
       </c>
@@ -2389,13 +2360,11 @@
           <t>ram.matlani@tatacapital.com</t>
         </is>
       </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>Sent email at slno 71 at time: 11/12/2025,18:04:23</t>
-        </is>
-      </c>
-    </row>
-    <row r="76" ht="15" customHeight="1" thickBot="1">
+      <c r="I75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" ht="15.75" customHeight="1" thickBot="1">
       <c r="C76" s="3" t="n">
         <v>72</v>
       </c>
@@ -2414,13 +2383,11 @@
           <t>deewakar.bhatt@cba.com.au</t>
         </is>
       </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>Sent email at slno 72 at time: 11/12/2025,18:04:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="77" ht="15" customHeight="1" thickBot="1">
+      <c r="I76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" ht="15.75" customHeight="1" thickBot="1">
       <c r="C77" s="3" t="n">
         <v>73</v>
       </c>
@@ -2439,13 +2406,11 @@
           <t>sachinn@hdfcsales.com</t>
         </is>
       </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>Sent email at slno 73 at time: 11/12/2025,18:04:35</t>
-        </is>
-      </c>
-    </row>
-    <row r="78" ht="15" customHeight="1" thickBot="1">
+      <c r="I77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" ht="15.75" customHeight="1" thickBot="1">
       <c r="C78" s="3" t="n">
         <v>74</v>
       </c>
@@ -2464,13 +2429,11 @@
           <t>shashank.saxena@pnbhousing.com</t>
         </is>
       </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>Sent email at slno 74 at time: 11/12/2025,18:04:40</t>
-        </is>
-      </c>
-    </row>
-    <row r="79" ht="15" customHeight="1" thickBot="1">
+      <c r="I78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" ht="15.75" customHeight="1" thickBot="1">
       <c r="C79" s="3" t="n">
         <v>75</v>
       </c>
@@ -2489,13 +2452,11 @@
           <t>abhishekj@hdfcsales.com</t>
         </is>
       </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>Sent email at slno 75 at time: 11/12/2025,18:04:46</t>
-        </is>
-      </c>
-    </row>
-    <row r="80" ht="15" customHeight="1" thickBot="1">
+      <c r="I79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" ht="15.75" customHeight="1" thickBot="1">
       <c r="C80" s="3" t="n">
         <v>76</v>
       </c>
@@ -2514,13 +2475,11 @@
           <t>raj.chauhan@aubank.in</t>
         </is>
       </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>Sent email at slno 76 at time: 11/12/2025,18:04:51</t>
-        </is>
-      </c>
-    </row>
-    <row r="81" ht="15" customHeight="1" thickBot="1">
+      <c r="I80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" ht="15.75" customHeight="1" thickBot="1">
       <c r="C81" s="3" t="n">
         <v>77</v>
       </c>
@@ -2539,13 +2498,11 @@
           <t>piyush.aggarwal@bajajfinserv.in</t>
         </is>
       </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>Sent email at slno 77 at time: 11/12/2025,18:04:58</t>
-        </is>
-      </c>
-    </row>
-    <row r="82" ht="15" customHeight="1" thickBot="1">
+      <c r="I81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" ht="15.75" customHeight="1" thickBot="1">
       <c r="C82" s="3" t="n">
         <v>78</v>
       </c>
@@ -2564,13 +2521,11 @@
           <t>vinod.chandran@esafbank.com</t>
         </is>
       </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>Sent email at slno 78 at time: 11/12/2025,18:05:02</t>
-        </is>
-      </c>
-    </row>
-    <row r="83" ht="15" customHeight="1" thickBot="1">
+      <c r="I82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" ht="15.75" customHeight="1" thickBot="1">
       <c r="C83" s="3" t="n">
         <v>79</v>
       </c>
@@ -2589,13 +2544,11 @@
           <t>sunil.maurya@emkayglobal.com</t>
         </is>
       </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>Sent email at slno 79 at time: 11/12/2025,18:05:07</t>
-        </is>
-      </c>
-    </row>
-    <row r="84" ht="15" customHeight="1" thickBot="1">
+      <c r="I83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" ht="15.75" customHeight="1" thickBot="1">
       <c r="C84" s="3" t="n">
         <v>80</v>
       </c>
@@ -2614,13 +2567,11 @@
           <t>rohith.reghunadhan@axisbank.com</t>
         </is>
       </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>Sent email at slno 80 at time: 11/12/2025,18:05:15</t>
-        </is>
-      </c>
-    </row>
-    <row r="85" ht="15" customHeight="1" thickBot="1">
+      <c r="I84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" ht="15.75" customHeight="1" thickBot="1">
       <c r="C85" s="3" t="n">
         <v>81</v>
       </c>
@@ -2639,13 +2590,11 @@
           <t>pprabhu@nse.co.in</t>
         </is>
       </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>Sent email at slno 81 at time: 11/12/2025,18:05:20</t>
-        </is>
-      </c>
-    </row>
-    <row r="86" ht="15" customHeight="1" thickBot="1">
+      <c r="I85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" ht="15.75" customHeight="1" thickBot="1">
       <c r="C86" s="3" t="n">
         <v>82</v>
       </c>
@@ -2664,13 +2613,11 @@
           <t>devashish.goswami@equifax.com</t>
         </is>
       </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>Sent email at slno 82 at time: 11/12/2025,18:05:25</t>
-        </is>
-      </c>
-    </row>
-    <row r="87" ht="15" customHeight="1" thickBot="1">
+      <c r="I86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" ht="15.75" customHeight="1" thickBot="1">
       <c r="C87" s="3" t="n">
         <v>83</v>
       </c>
@@ -2689,13 +2636,11 @@
           <t>toyoja@flobiz.in</t>
         </is>
       </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>Sent email at slno 83 at time: 11/12/2025,18:05:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="88" ht="15" customHeight="1" thickBot="1">
+      <c r="I87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" ht="15.75" customHeight="1" thickBot="1">
       <c r="C88" s="3" t="n">
         <v>84</v>
       </c>
@@ -2714,13 +2659,11 @@
           <t>bharathyjagannathan@gmail.com</t>
         </is>
       </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>Sent email at slno 84 at time: 11/12/2025,18:05:37</t>
-        </is>
-      </c>
-    </row>
-    <row r="89" ht="15" customHeight="1" thickBot="1">
+      <c r="I88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" ht="15.75" customHeight="1" thickBot="1">
       <c r="C89" s="3" t="n">
         <v>85</v>
       </c>
@@ -2739,13 +2682,11 @@
           <t>pranita.jha@indusind.com</t>
         </is>
       </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>Sent email at slno 85 at time: 11/12/2025,18:05:43</t>
-        </is>
-      </c>
-    </row>
-    <row r="90" ht="15" customHeight="1" thickBot="1">
+      <c r="I89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" ht="15.75" customHeight="1" thickBot="1">
       <c r="C90" s="3" t="n">
         <v>86</v>
       </c>
@@ -2764,13 +2705,11 @@
           <t>harshal.shah@xldynamics.com</t>
         </is>
       </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>Sent email at slno 86 at time: 11/12/2025,18:05:50</t>
-        </is>
-      </c>
-    </row>
-    <row r="91" ht="15" customHeight="1" thickBot="1">
+      <c r="I90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" ht="15.75" customHeight="1" thickBot="1">
       <c r="C91" s="3" t="n">
         <v>87</v>
       </c>
@@ -2789,13 +2728,11 @@
           <t>ritika.pareek@aubank.in</t>
         </is>
       </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>Sent email at slno 87 at time: 11/12/2025,18:05:57</t>
-        </is>
-      </c>
-    </row>
-    <row r="92" ht="15" customHeight="1" thickBot="1">
+      <c r="I91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" ht="15.75" customHeight="1" thickBot="1">
       <c r="C92" s="3" t="n">
         <v>88</v>
       </c>
@@ -2814,13 +2751,11 @@
           <t>saurabh.awasthy@bandhanbank.com</t>
         </is>
       </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>Sent email at slno 88 at time: 11/12/2025,18:06:02</t>
-        </is>
-      </c>
-    </row>
-    <row r="93" ht="15" customHeight="1" thickBot="1">
+      <c r="I92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" ht="15.75" customHeight="1" thickBot="1">
       <c r="C93" s="3" t="n">
         <v>89</v>
       </c>
@@ -2839,13 +2774,11 @@
           <t>roshan.shilimkar@janabank.com</t>
         </is>
       </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>Sent email at slno 89 at time: 11/12/2025,18:06:07</t>
-        </is>
-      </c>
-    </row>
-    <row r="94" ht="15" customHeight="1" thickBot="1">
+      <c r="I93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" ht="15.75" customHeight="1" thickBot="1">
       <c r="C94" s="3" t="n">
         <v>90</v>
       </c>
@@ -2864,13 +2797,11 @@
           <t>dayashankar@muthootmicrofin.com</t>
         </is>
       </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>Sent email at slno 90 at time: 11/12/2025,18:06:12</t>
-        </is>
-      </c>
-    </row>
-    <row r="95" ht="15" customHeight="1" thickBot="1">
+      <c r="I94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" ht="15.75" customHeight="1" thickBot="1">
       <c r="C95" s="3" t="n">
         <v>91</v>
       </c>
@@ -2889,13 +2820,11 @@
           <t>fawad.khot@kotak.com</t>
         </is>
       </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>Sent email at slno 91 at time: 11/12/2025,18:06:17</t>
-        </is>
-      </c>
-    </row>
-    <row r="96" ht="15" customHeight="1" thickBot="1">
+      <c r="I95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" ht="15.75" customHeight="1" thickBot="1">
       <c r="C96" s="3" t="n">
         <v>92</v>
       </c>
@@ -2914,17 +2843,25 @@
           <t>kushankur.mukherjee@bandhanbank.com</t>
         </is>
       </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>Sent email at slno 92 at time: 11/12/2025,18:06:22</t>
-        </is>
+      <c r="I96" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F7" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O3" display="mailto:apoorva.patil@tcs.com" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O4" display="mailto:prashant.kothari@airindiaexpress.in" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O5" display="mailto:nidhika.abrol@rjcorp.in" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O6" display="mailto:monideepa.j@tataconsumer.com" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F7" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O7" display="mailto:rkc@apac.ko.com" r:id="rId8"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O8" display="mailto:vishal.dey@hdfcergo.com" r:id="rId9"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O10" display="mailto:meenal.gupta@bajajallianz.co.in" r:id="rId10"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O11" display="mailto:vishwachandrannair@iiflsamasta.com" r:id="rId11"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O13" display="mailto:rishi.raghuvanshi@ujjivan.com" r:id="rId12"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O15" display="mailto:raghavg@vfsglobal.com" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>